<commit_message>
Create Scheduling Driven loop
</commit_message>
<xml_diff>
--- a/Scheduling.xlsx
+++ b/Scheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7578EE8B-B00F-4AA5-8B99-F8ABF83CEE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E7A92-646F-46CE-9E64-DA4687CACB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25650" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{92B48E2A-042F-4F36-80C7-1DF77AAA5046}"/>
+    <workbookView xWindow="6150" yWindow="3930" windowWidth="21600" windowHeight="11385" xr2:uid="{92B48E2A-042F-4F36-80C7-1DF77AAA5046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,34 +36,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>External No</t>
-  </si>
-  <si>
-    <t>Group ID</t>
-  </si>
-  <si>
-    <t>Requested date/time</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>4 - Medium</t>
-  </si>
-  <si>
-    <t>Type of transport</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>25/01/2025</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>20/01/2025</t>
+  </si>
+  <si>
+    <t>21/01/2025</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>19/01/2025</t>
+  </si>
+  <si>
+    <t>17/01/2025</t>
+  </si>
+  <si>
+    <t>15/01/2025</t>
+  </si>
+  <si>
+    <t>Order template</t>
+  </si>
+  <si>
+    <t>Cardioversion</t>
+  </si>
+  <si>
+    <t>Echokardiographie TTE</t>
+  </si>
+  <si>
+    <t>Ultrasound [US] (DCM01)</t>
+  </si>
+  <si>
+    <t>MRT (DCM03)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,52 +463,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D80F35-143B-406B-A660-04C4D7774C53}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1000000008</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1000000003</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.35416666666666702</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1000000421</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1000000005</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>123</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="F5" s="1">
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>